<commit_message>
Ajustes de fotos, hospedaje
</commit_message>
<xml_diff>
--- a/excelconcodigos.xlsx
+++ b/excelconcodigos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriaandrade/Desktop/Invitacion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B0F608-3664-DB48-B986-56FD41634294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE080E7-0A69-E747-B25E-FBE995FA8BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7020" yWindow="4160" windowWidth="26040" windowHeight="13820" xr2:uid="{1736CF8A-6106-FD44-BB74-70597C00E89D}"/>
   </bookViews>
@@ -939,7 +939,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>